<commit_message>
fixed sending e-mails with an update of the gains/losses
</commit_message>
<xml_diff>
--- a/stock_data.xlsx
+++ b/stock_data.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
@@ -658,6 +658,774 @@
         <v>84.50704225352113</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RDZN</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-3.286384976525814</v>
+      </c>
+      <c r="F8" t="n">
+        <v>96.71361502347419</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>VS</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.362204724409451</v>
+      </c>
+      <c r="F9" t="n">
+        <v>102.3622047244095</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>GMM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RDZN</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-3.286384976525814</v>
+      </c>
+      <c r="F11" t="n">
+        <v>96.71361502347419</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>VS</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.362204724409451</v>
+      </c>
+      <c r="F12" t="n">
+        <v>102.3622047244095</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>GMM</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>RDZN</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-3.286384976525814</v>
+      </c>
+      <c r="F14" t="n">
+        <v>96.71361502347419</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>VS</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.362204724409451</v>
+      </c>
+      <c r="F15" t="n">
+        <v>102.3622047244095</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>GMM</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>RDZN</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-3.286384976525814</v>
+      </c>
+      <c r="F17" t="n">
+        <v>96.71361502347419</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>VS</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.362204724409451</v>
+      </c>
+      <c r="F18" t="n">
+        <v>102.3622047244095</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>GMM</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>RDZN</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-3.286384976525814</v>
+      </c>
+      <c r="F20" t="n">
+        <v>96.71361502347419</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>VS</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2.362204724409451</v>
+      </c>
+      <c r="F21" t="n">
+        <v>102.3622047244095</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GMM</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D23" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F23" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D24" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F24" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D25" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F25" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D26" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F26" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D27" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F27" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D28" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F28" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D29" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F29" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D30" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F30" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D31" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F31" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D32" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F32" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D33" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F33" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D34" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F34" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D35" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F35" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D36" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F36" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D37" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F37" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D38" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F38" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>173.45</v>
+      </c>
+      <c r="D39" t="n">
+        <v>173.81</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.2075526088209937</v>
+      </c>
+      <c r="F39" t="n">
+        <v>100.207552608821</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>